<commit_message>
Kế hoạch làm việc
</commit_message>
<xml_diff>
--- a/Project_Plan.xlsx
+++ b/Project_Plan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="39">
   <si>
     <t>TASK</t>
   </si>
@@ -132,9 +132,6 @@
   </si>
   <si>
     <t>27/10</t>
-  </si>
-  <si>
-    <t>In Progress</t>
   </si>
   <si>
     <t>Not Started</t>
@@ -150,7 +147,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,13 +167,6 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="7" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -233,15 +223,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -250,7 +237,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -539,26 +526,26 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9:F11"/>
+      <selection activeCell="F9" sqref="F9:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.75" customWidth="1"/>
-    <col min="2" max="2" width="18.625" customWidth="1"/>
-    <col min="3" max="3" width="8.125" customWidth="1"/>
-    <col min="6" max="6" width="11.5" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
+      <c r="A1" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -596,8 +583,8 @@
       <c r="E3" s="2">
         <v>5</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>39</v>
+      <c r="F3" s="5" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -616,8 +603,8 @@
       <c r="E4" s="2">
         <v>4</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>39</v>
+      <c r="F4" s="5" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -636,8 +623,8 @@
       <c r="E5" s="2">
         <v>5</v>
       </c>
-      <c r="F5" s="6" t="s">
-        <v>39</v>
+      <c r="F5" s="5" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -656,8 +643,8 @@
       <c r="E6" s="2">
         <v>7</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>39</v>
+      <c r="F6" s="5" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -676,8 +663,8 @@
       <c r="E7" s="2">
         <v>1</v>
       </c>
-      <c r="F7" s="6" t="s">
-        <v>39</v>
+      <c r="F7" s="5" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -696,8 +683,8 @@
       <c r="E8" s="2">
         <v>20</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>39</v>
+      <c r="F8" s="5" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -716,8 +703,8 @@
       <c r="E9" s="2">
         <v>20</v>
       </c>
-      <c r="F9" s="6" t="s">
-        <v>39</v>
+      <c r="F9" s="5" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -736,8 +723,8 @@
       <c r="E10" s="2">
         <v>20</v>
       </c>
-      <c r="F10" s="6" t="s">
-        <v>39</v>
+      <c r="F10" s="5" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -756,8 +743,8 @@
       <c r="E11" s="2">
         <v>1</v>
       </c>
-      <c r="F11" s="6" t="s">
-        <v>39</v>
+      <c r="F11" s="5" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -776,26 +763,26 @@
       <c r="E12" s="2">
         <v>7</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="3">
+        <v>1</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="4">
-        <v>1</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>